<commit_message>
Updated Excel and Word + first ocr prototype (not working yet)
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidkapka/blj-notewriter/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6303E7FA-A063-D649-B36D-7AAFA46219AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D3B4E0-9EBC-0641-9557-43748A2B4821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -86,6 +86,7 @@
             <color rgb="FF000000"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Besprechung Anforderungsanalyse-Dokument (mit Urs/Kilian)
 </t>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>Nr.</t>
   </si>
@@ -249,9 +250,6 @@
     <t>KW 53</t>
   </si>
   <si>
-    <t>Anforderung NF001</t>
-  </si>
-  <si>
     <t>Anforderung A001</t>
   </si>
   <si>
@@ -267,16 +265,13 @@
     <t>Anforderung A004</t>
   </si>
   <si>
-    <t>Anforderung A006</t>
-  </si>
-  <si>
-    <t>Anforderung A007</t>
-  </si>
-  <si>
     <t>NoteWriter+</t>
   </si>
   <si>
     <t>Anforderung A003</t>
+  </si>
+  <si>
+    <t>Anforderung NF001 &amp; NF002</t>
   </si>
 </sst>
 </file>
@@ -374,12 +369,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
@@ -391,6 +380,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1144,7 +1140,7 @@
     </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1453,7 +1449,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1494,14 +1490,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1547,6 +1535,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1651,10 +1654,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
@@ -1725,7 +1728,7 @@
                   <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.75</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -2235,8 +2238,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2252,7 +2255,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="25" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2555,88 +2558,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="108"/>
+      <c r="D7" s="106"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="109" t="s">
+      <c r="G7" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="109" t="s">
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="109"/>
-      <c r="P7" s="109"/>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="109"/>
-      <c r="S7" s="109"/>
-      <c r="T7" s="110"/>
-      <c r="U7" s="109" t="s">
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="107"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="V7" s="109"/>
-      <c r="W7" s="109"/>
-      <c r="X7" s="109"/>
-      <c r="Y7" s="109"/>
-      <c r="Z7" s="109"/>
-      <c r="AA7" s="110"/>
-      <c r="AB7" s="111" t="s">
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="107"/>
+      <c r="Y7" s="107"/>
+      <c r="Z7" s="107"/>
+      <c r="AA7" s="108"/>
+      <c r="AB7" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="AC7" s="109"/>
-      <c r="AD7" s="109"/>
-      <c r="AE7" s="109"/>
-      <c r="AF7" s="109"/>
-      <c r="AG7" s="109"/>
-      <c r="AH7" s="110"/>
-      <c r="AI7" s="109" t="s">
+      <c r="AC7" s="107"/>
+      <c r="AD7" s="107"/>
+      <c r="AE7" s="107"/>
+      <c r="AF7" s="107"/>
+      <c r="AG7" s="107"/>
+      <c r="AH7" s="108"/>
+      <c r="AI7" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="AJ7" s="109"/>
-      <c r="AK7" s="109"/>
-      <c r="AL7" s="109"/>
-      <c r="AM7" s="109"/>
-      <c r="AN7" s="109"/>
-      <c r="AO7" s="110"/>
-      <c r="AP7" s="111" t="s">
+      <c r="AJ7" s="107"/>
+      <c r="AK7" s="107"/>
+      <c r="AL7" s="107"/>
+      <c r="AM7" s="107"/>
+      <c r="AN7" s="107"/>
+      <c r="AO7" s="108"/>
+      <c r="AP7" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="AQ7" s="109"/>
-      <c r="AR7" s="109"/>
-      <c r="AS7" s="109"/>
-      <c r="AT7" s="109"/>
-      <c r="AU7" s="109"/>
-      <c r="AV7" s="110"/>
-      <c r="AW7" s="109" t="s">
+      <c r="AQ7" s="107"/>
+      <c r="AR7" s="107"/>
+      <c r="AS7" s="107"/>
+      <c r="AT7" s="107"/>
+      <c r="AU7" s="107"/>
+      <c r="AV7" s="108"/>
+      <c r="AW7" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="AX7" s="109"/>
-      <c r="AY7" s="109"/>
-      <c r="AZ7" s="109"/>
-      <c r="BA7" s="109"/>
-      <c r="BB7" s="109"/>
-      <c r="BC7" s="110"/>
-      <c r="BD7" s="111" t="s">
+      <c r="AX7" s="107"/>
+      <c r="AY7" s="107"/>
+      <c r="AZ7" s="107"/>
+      <c r="BA7" s="107"/>
+      <c r="BB7" s="107"/>
+      <c r="BC7" s="108"/>
+      <c r="BD7" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="BE7" s="109"/>
-      <c r="BF7" s="109"/>
-      <c r="BG7" s="109"/>
-      <c r="BH7" s="109"/>
-      <c r="BI7" s="109"/>
-      <c r="BJ7" s="112"/>
+      <c r="BE7" s="107"/>
+      <c r="BF7" s="107"/>
+      <c r="BG7" s="107"/>
+      <c r="BH7" s="107"/>
+      <c r="BI7" s="107"/>
+      <c r="BJ7" s="110"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -2938,15 +2941,15 @@
       <c r="AA10" s="58"/>
       <c r="AB10" s="98"/>
       <c r="AC10" s="99"/>
-      <c r="AD10" s="105"/>
-      <c r="AE10" s="105"/>
+      <c r="AD10" s="103"/>
+      <c r="AE10" s="103"/>
       <c r="AF10" s="57"/>
       <c r="AG10" s="57"/>
       <c r="AH10" s="58"/>
       <c r="AI10" s="53"/>
       <c r="AJ10" s="54"/>
-      <c r="AK10" s="105"/>
-      <c r="AL10" s="105"/>
+      <c r="AK10" s="103"/>
+      <c r="AL10" s="103"/>
       <c r="AM10" s="57"/>
       <c r="AN10" s="57"/>
       <c r="AO10" s="58"/>
@@ -3168,16 +3171,16 @@
       <c r="AA13" s="67"/>
       <c r="AB13" s="100"/>
       <c r="AC13" s="61"/>
-      <c r="AD13" s="105"/>
-      <c r="AE13" s="105"/>
-      <c r="AF13" s="105"/>
+      <c r="AD13" s="103"/>
+      <c r="AE13" s="103"/>
+      <c r="AF13" s="103"/>
       <c r="AG13" s="66"/>
       <c r="AH13" s="67"/>
       <c r="AI13" s="59"/>
       <c r="AJ13" s="60"/>
-      <c r="AK13" s="105"/>
-      <c r="AL13" s="105"/>
-      <c r="AM13" s="105"/>
+      <c r="AK13" s="103"/>
+      <c r="AL13" s="103"/>
+      <c r="AM13" s="103"/>
       <c r="AN13" s="66"/>
       <c r="AO13" s="67"/>
       <c r="AP13" s="59"/>
@@ -3211,11 +3214,11 @@
       </c>
       <c r="C14" s="41">
         <f>SUM(C15:C17)</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3284,11 +3287,11 @@
         <v>26</v>
       </c>
       <c r="C15" s="49">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D15" s="82">
         <f>SUM(G15:BJ15)</f>
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="88" t="s">
@@ -3300,7 +3303,9 @@
       <c r="J15" s="93">
         <v>0.75</v>
       </c>
-      <c r="K15" s="86"/>
+      <c r="K15" s="86">
+        <v>0.5</v>
+      </c>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
       <c r="N15" s="53"/>
@@ -3319,15 +3324,15 @@
       <c r="AA15" s="58"/>
       <c r="AB15" s="98"/>
       <c r="AC15" s="99"/>
-      <c r="AD15" s="105"/>
-      <c r="AE15" s="105"/>
+      <c r="AD15" s="103"/>
+      <c r="AE15" s="103"/>
       <c r="AF15" s="57"/>
       <c r="AG15" s="57"/>
       <c r="AH15" s="58"/>
       <c r="AI15" s="53"/>
       <c r="AJ15" s="54"/>
-      <c r="AK15" s="105"/>
-      <c r="AL15" s="105"/>
+      <c r="AK15" s="103"/>
+      <c r="AL15" s="103"/>
       <c r="AM15" s="57"/>
       <c r="AN15" s="57"/>
       <c r="AO15" s="58"/>
@@ -3394,15 +3399,15 @@
       <c r="AA16" s="58"/>
       <c r="AB16" s="100"/>
       <c r="AC16" s="61"/>
-      <c r="AD16" s="105"/>
-      <c r="AE16" s="105"/>
+      <c r="AD16" s="103"/>
+      <c r="AE16" s="103"/>
       <c r="AF16" s="57"/>
       <c r="AG16" s="57"/>
       <c r="AH16" s="58"/>
       <c r="AI16" s="59"/>
       <c r="AJ16" s="60"/>
-      <c r="AK16" s="105"/>
-      <c r="AL16" s="105"/>
+      <c r="AK16" s="103"/>
+      <c r="AL16" s="103"/>
       <c r="AM16" s="57"/>
       <c r="AN16" s="57"/>
       <c r="AO16" s="58"/>
@@ -3463,15 +3468,15 @@
       <c r="AA17" s="58"/>
       <c r="AB17" s="101"/>
       <c r="AC17" s="102"/>
-      <c r="AD17" s="105"/>
-      <c r="AE17" s="105"/>
+      <c r="AD17" s="103"/>
+      <c r="AE17" s="103"/>
       <c r="AF17" s="57"/>
       <c r="AG17" s="57"/>
       <c r="AH17" s="58"/>
       <c r="AI17" s="68"/>
       <c r="AJ17" s="69"/>
-      <c r="AK17" s="105"/>
-      <c r="AL17" s="105"/>
+      <c r="AK17" s="103"/>
+      <c r="AL17" s="103"/>
       <c r="AM17" s="57"/>
       <c r="AN17" s="57"/>
       <c r="AO17" s="58"/>
@@ -3506,7 +3511,7 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
@@ -3616,15 +3621,15 @@
       <c r="AA19" s="58"/>
       <c r="AB19" s="98"/>
       <c r="AC19" s="99"/>
-      <c r="AD19" s="105"/>
-      <c r="AE19" s="105"/>
+      <c r="AD19" s="103"/>
+      <c r="AE19" s="103"/>
       <c r="AF19" s="57"/>
       <c r="AG19" s="57"/>
       <c r="AH19" s="58"/>
       <c r="AI19" s="53"/>
       <c r="AJ19" s="54"/>
-      <c r="AK19" s="105"/>
-      <c r="AL19" s="105"/>
+      <c r="AK19" s="103"/>
+      <c r="AL19" s="103"/>
       <c r="AM19" s="57"/>
       <c r="AN19" s="57"/>
       <c r="AO19" s="58"/>
@@ -3691,15 +3696,15 @@
       <c r="AA20" s="58"/>
       <c r="AB20" s="100"/>
       <c r="AC20" s="61"/>
-      <c r="AD20" s="105"/>
-      <c r="AE20" s="105"/>
+      <c r="AD20" s="103"/>
+      <c r="AE20" s="103"/>
       <c r="AF20" s="57"/>
       <c r="AG20" s="57"/>
       <c r="AH20" s="58"/>
       <c r="AI20" s="59"/>
       <c r="AJ20" s="60"/>
-      <c r="AK20" s="105"/>
-      <c r="AL20" s="105"/>
+      <c r="AK20" s="103"/>
+      <c r="AL20" s="103"/>
       <c r="AM20" s="57"/>
       <c r="AN20" s="57"/>
       <c r="AO20" s="58"/>
@@ -3730,10 +3735,10 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C21" s="49">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D21" s="82">
         <f t="shared" si="0"/>
@@ -3766,15 +3771,15 @@
       <c r="AA21" s="58"/>
       <c r="AB21" s="100"/>
       <c r="AC21" s="61"/>
-      <c r="AD21" s="105"/>
-      <c r="AE21" s="105"/>
+      <c r="AD21" s="103"/>
+      <c r="AE21" s="103"/>
       <c r="AF21" s="57"/>
       <c r="AG21" s="57"/>
       <c r="AH21" s="58"/>
       <c r="AI21" s="59"/>
       <c r="AJ21" s="60"/>
-      <c r="AK21" s="105"/>
-      <c r="AL21" s="105"/>
+      <c r="AK21" s="103"/>
+      <c r="AL21" s="103"/>
       <c r="AM21" s="57"/>
       <c r="AN21" s="57"/>
       <c r="AO21" s="58"/>
@@ -3805,7 +3810,7 @@
         <v>304</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="49">
         <v>8</v>
@@ -3828,28 +3833,27 @@
       <c r="N22" s="59"/>
       <c r="O22" s="60"/>
       <c r="P22" s="96"/>
-      <c r="Q22" s="93"/>
-      <c r="R22" s="94"/>
+      <c r="R22" s="93"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="96"/>
+      <c r="W22" s="93"/>
       <c r="X22" s="96"/>
       <c r="Y22" s="97"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
       <c r="AB22" s="100"/>
       <c r="AC22" s="61"/>
-      <c r="AD22" s="105"/>
-      <c r="AE22" s="105"/>
+      <c r="AD22" s="103"/>
+      <c r="AE22" s="103"/>
       <c r="AF22" s="57"/>
       <c r="AG22" s="57"/>
       <c r="AH22" s="58"/>
       <c r="AI22" s="59"/>
       <c r="AJ22" s="60"/>
-      <c r="AK22" s="105"/>
-      <c r="AL22" s="105"/>
+      <c r="AK22" s="103"/>
+      <c r="AL22" s="103"/>
       <c r="AM22" s="57"/>
       <c r="AN22" s="57"/>
       <c r="AO22" s="58"/>
@@ -3883,7 +3887,7 @@
         <v>52</v>
       </c>
       <c r="C23" s="49">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D23" s="82">
         <f t="shared" si="0"/>
@@ -3910,7 +3914,7 @@
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
       <c r="W23" s="95"/>
-      <c r="X23" s="84"/>
+      <c r="X23" s="95"/>
       <c r="Y23" s="97"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
@@ -3955,10 +3959,10 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C24" s="49">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D24" s="82">
         <f t="shared" si="0"/>
@@ -3984,22 +3988,22 @@
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
-      <c r="W24" s="93"/>
+      <c r="W24" s="96"/>
       <c r="X24" s="93"/>
-      <c r="Y24" s="97"/>
+      <c r="Y24" s="94"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
-      <c r="AB24" s="100"/>
-      <c r="AC24" s="61"/>
-      <c r="AD24" s="105"/>
-      <c r="AE24" s="105"/>
+      <c r="AB24" s="104"/>
+      <c r="AC24" s="84"/>
+      <c r="AD24" s="103"/>
+      <c r="AE24" s="103"/>
       <c r="AF24" s="57"/>
       <c r="AG24" s="57"/>
       <c r="AH24" s="58"/>
       <c r="AI24" s="59"/>
       <c r="AJ24" s="60"/>
-      <c r="AK24" s="105"/>
-      <c r="AL24" s="105"/>
+      <c r="AK24" s="103"/>
+      <c r="AL24" s="103"/>
       <c r="AM24" s="57"/>
       <c r="AN24" s="57"/>
       <c r="AO24" s="58"/>
@@ -4030,10 +4034,10 @@
         <v>307</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C25" s="49">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D25" s="82">
         <f t="shared" si="0"/>
@@ -4061,20 +4065,20 @@
       <c r="V25" s="60"/>
       <c r="W25" s="96"/>
       <c r="X25" s="96"/>
-      <c r="Y25" s="94"/>
+      <c r="Y25" s="97"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
-      <c r="AB25" s="106"/>
-      <c r="AC25" s="84"/>
-      <c r="AD25" s="105"/>
-      <c r="AE25" s="105"/>
+      <c r="AB25" s="104"/>
+      <c r="AC25" s="95"/>
+      <c r="AD25" s="103"/>
+      <c r="AE25" s="103"/>
       <c r="AF25" s="57"/>
       <c r="AG25" s="57"/>
       <c r="AH25" s="58"/>
       <c r="AI25" s="59"/>
       <c r="AJ25" s="60"/>
-      <c r="AK25" s="105"/>
-      <c r="AL25" s="105"/>
+      <c r="AK25" s="103"/>
+      <c r="AL25" s="103"/>
       <c r="AM25" s="57"/>
       <c r="AN25" s="57"/>
       <c r="AO25" s="58"/>
@@ -4108,7 +4112,7 @@
         <v>54</v>
       </c>
       <c r="C26" s="49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" s="82">
         <f t="shared" si="0"/>
@@ -4137,23 +4141,23 @@
       <c r="Y26" s="56"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
-      <c r="AB26" s="106"/>
+      <c r="AB26" s="115"/>
       <c r="AC26" s="84"/>
-      <c r="AD26" s="105"/>
-      <c r="AE26" s="105"/>
+      <c r="AD26" s="103"/>
+      <c r="AE26" s="103"/>
       <c r="AF26" s="57"/>
       <c r="AG26" s="57"/>
       <c r="AH26" s="58"/>
       <c r="AI26" s="59"/>
       <c r="AJ26" s="60"/>
-      <c r="AK26" s="105"/>
-      <c r="AL26" s="105"/>
+      <c r="AK26" s="103"/>
+      <c r="AL26" s="103"/>
       <c r="AM26" s="57"/>
       <c r="AN26" s="57"/>
       <c r="AO26" s="58"/>
       <c r="AP26" s="59"/>
       <c r="AQ26" s="60"/>
-      <c r="AR26" s="55"/>
+      <c r="AR26" s="93"/>
       <c r="AS26" s="55"/>
       <c r="AT26" s="56"/>
       <c r="AU26" s="57"/>
@@ -4178,10 +4182,10 @@
         <v>309</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C27" s="49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="82">
         <f t="shared" si="0"/>
@@ -4210,23 +4214,24 @@
       <c r="Y27" s="56"/>
       <c r="Z27" s="57"/>
       <c r="AA27" s="58"/>
-      <c r="AC27" s="106"/>
-      <c r="AD27" s="105"/>
-      <c r="AE27" s="105"/>
+      <c r="AB27" s="116"/>
+      <c r="AC27" s="115"/>
+      <c r="AD27" s="103"/>
+      <c r="AE27" s="103"/>
       <c r="AF27" s="57"/>
       <c r="AG27" s="57"/>
       <c r="AH27" s="58"/>
       <c r="AI27" s="59"/>
       <c r="AJ27" s="60"/>
-      <c r="AK27" s="105"/>
-      <c r="AL27" s="105"/>
+      <c r="AK27" s="103"/>
+      <c r="AL27" s="103"/>
       <c r="AM27" s="57"/>
       <c r="AN27" s="57"/>
       <c r="AO27" s="58"/>
       <c r="AP27" s="59"/>
       <c r="AQ27" s="60"/>
       <c r="AR27" s="55"/>
-      <c r="AS27" s="55"/>
+      <c r="AS27" s="93"/>
       <c r="AT27" s="56"/>
       <c r="AU27" s="57"/>
       <c r="AV27" s="58"/>
@@ -4249,12 +4254,8 @@
       <c r="A28" s="12">
         <v>310</v>
       </c>
-      <c r="B28" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="49">
-        <v>3</v>
-      </c>
+      <c r="B28" s="46"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4282,23 +4283,23 @@
       <c r="Y28" s="56"/>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
-      <c r="AB28" s="100"/>
-      <c r="AC28" s="95"/>
-      <c r="AD28" s="105"/>
-      <c r="AE28" s="105"/>
+      <c r="AB28" s="115"/>
+      <c r="AC28" s="84"/>
+      <c r="AD28" s="103"/>
+      <c r="AE28" s="103"/>
       <c r="AF28" s="57"/>
       <c r="AG28" s="57"/>
       <c r="AH28" s="58"/>
       <c r="AI28" s="59"/>
       <c r="AJ28" s="60"/>
-      <c r="AK28" s="105"/>
-      <c r="AL28" s="105"/>
+      <c r="AK28" s="103"/>
+      <c r="AL28" s="103"/>
       <c r="AM28" s="57"/>
       <c r="AN28" s="57"/>
       <c r="AO28" s="58"/>
       <c r="AP28" s="59"/>
       <c r="AQ28" s="60"/>
-      <c r="AR28" s="55"/>
+      <c r="AR28" s="96"/>
       <c r="AS28" s="55"/>
       <c r="AT28" s="56"/>
       <c r="AU28" s="57"/>
@@ -4322,12 +4323,8 @@
       <c r="A29" s="12">
         <v>311</v>
       </c>
-      <c r="B29" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="49">
-        <v>5</v>
-      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4355,23 +4352,23 @@
       <c r="Y29" s="56"/>
       <c r="Z29" s="57"/>
       <c r="AA29" s="58"/>
-      <c r="AB29" s="103"/>
-      <c r="AC29" s="104"/>
-      <c r="AD29" s="105"/>
-      <c r="AE29" s="105"/>
+      <c r="AB29" s="117"/>
+      <c r="AC29" s="118"/>
+      <c r="AD29" s="103"/>
+      <c r="AE29" s="103"/>
       <c r="AF29" s="57"/>
       <c r="AG29" s="57"/>
       <c r="AH29" s="58"/>
       <c r="AI29" s="70"/>
       <c r="AJ29" s="71"/>
-      <c r="AK29" s="105"/>
-      <c r="AL29" s="105"/>
+      <c r="AK29" s="103"/>
+      <c r="AL29" s="103"/>
       <c r="AM29" s="57"/>
       <c r="AN29" s="57"/>
       <c r="AO29" s="58"/>
       <c r="AP29" s="70"/>
       <c r="AQ29" s="71"/>
-      <c r="AR29" s="93"/>
+      <c r="AR29" s="96"/>
       <c r="AS29" s="55"/>
       <c r="AT29" s="56"/>
       <c r="AU29" s="57"/>
@@ -4426,15 +4423,15 @@
       <c r="AA30" s="58"/>
       <c r="AB30" s="101"/>
       <c r="AC30" s="102"/>
-      <c r="AD30" s="105"/>
-      <c r="AE30" s="105"/>
+      <c r="AD30" s="103"/>
+      <c r="AE30" s="103"/>
       <c r="AF30" s="57"/>
       <c r="AG30" s="57"/>
       <c r="AH30" s="58"/>
       <c r="AI30" s="68"/>
       <c r="AJ30" s="69"/>
-      <c r="AK30" s="105"/>
-      <c r="AL30" s="105"/>
+      <c r="AK30" s="103"/>
+      <c r="AL30" s="103"/>
       <c r="AM30" s="57"/>
       <c r="AN30" s="57"/>
       <c r="AO30" s="58"/>
@@ -4572,16 +4569,16 @@
       <c r="Z32" s="57"/>
       <c r="AA32" s="58"/>
       <c r="AB32" s="98"/>
-      <c r="AC32" s="107"/>
-      <c r="AD32" s="105"/>
-      <c r="AE32" s="105"/>
+      <c r="AC32" s="105"/>
+      <c r="AD32" s="103"/>
+      <c r="AE32" s="103"/>
       <c r="AF32" s="57"/>
       <c r="AG32" s="57"/>
       <c r="AH32" s="58"/>
       <c r="AI32" s="53"/>
       <c r="AJ32" s="54"/>
-      <c r="AK32" s="105"/>
-      <c r="AL32" s="105"/>
+      <c r="AK32" s="103"/>
+      <c r="AL32" s="103"/>
       <c r="AM32" s="57"/>
       <c r="AN32" s="57"/>
       <c r="AO32" s="58"/>
@@ -4646,15 +4643,15 @@
       <c r="AA33" s="58"/>
       <c r="AB33" s="100"/>
       <c r="AC33" s="95"/>
-      <c r="AD33" s="105"/>
-      <c r="AE33" s="105"/>
+      <c r="AD33" s="103"/>
+      <c r="AE33" s="103"/>
       <c r="AF33" s="57"/>
       <c r="AG33" s="57"/>
       <c r="AH33" s="58"/>
       <c r="AI33" s="59"/>
       <c r="AJ33" s="60"/>
-      <c r="AK33" s="105"/>
-      <c r="AL33" s="105"/>
+      <c r="AK33" s="103"/>
+      <c r="AL33" s="103"/>
       <c r="AM33" s="57"/>
       <c r="AN33" s="57"/>
       <c r="AO33" s="58"/>
@@ -4719,15 +4716,15 @@
       <c r="AA34" s="58"/>
       <c r="AB34" s="100"/>
       <c r="AC34" s="95"/>
-      <c r="AD34" s="105"/>
-      <c r="AE34" s="105"/>
+      <c r="AD34" s="103"/>
+      <c r="AE34" s="103"/>
       <c r="AF34" s="57"/>
       <c r="AG34" s="57"/>
       <c r="AH34" s="58"/>
       <c r="AI34" s="59"/>
       <c r="AJ34" s="60"/>
-      <c r="AK34" s="105"/>
-      <c r="AL34" s="105"/>
+      <c r="AK34" s="103"/>
+      <c r="AL34" s="103"/>
       <c r="AM34" s="57"/>
       <c r="AN34" s="57"/>
       <c r="AO34" s="58"/>
@@ -4788,15 +4785,15 @@
       <c r="AA35" s="58"/>
       <c r="AB35" s="101"/>
       <c r="AC35" s="102"/>
-      <c r="AD35" s="105"/>
-      <c r="AE35" s="105"/>
+      <c r="AD35" s="103"/>
+      <c r="AE35" s="103"/>
       <c r="AF35" s="57"/>
       <c r="AG35" s="57"/>
       <c r="AH35" s="58"/>
       <c r="AI35" s="68"/>
       <c r="AJ35" s="69"/>
-      <c r="AK35" s="105"/>
-      <c r="AL35" s="105"/>
+      <c r="AK35" s="103"/>
+      <c r="AL35" s="103"/>
       <c r="AM35" s="57"/>
       <c r="AN35" s="57"/>
       <c r="AO35" s="58"/>
@@ -4933,15 +4930,15 @@
       <c r="AA37" s="58"/>
       <c r="AB37" s="98"/>
       <c r="AC37" s="99"/>
-      <c r="AD37" s="105"/>
-      <c r="AE37" s="105"/>
+      <c r="AD37" s="103"/>
+      <c r="AE37" s="103"/>
       <c r="AF37" s="57"/>
       <c r="AG37" s="57"/>
       <c r="AH37" s="58"/>
       <c r="AI37" s="53"/>
       <c r="AJ37" s="54"/>
-      <c r="AK37" s="105"/>
-      <c r="AL37" s="105"/>
+      <c r="AK37" s="103"/>
+      <c r="AL37" s="103"/>
       <c r="AM37" s="57"/>
       <c r="AN37" s="57"/>
       <c r="AO37" s="58"/>
@@ -5002,15 +4999,15 @@
       <c r="AA38" s="58"/>
       <c r="AB38" s="101"/>
       <c r="AC38" s="102"/>
-      <c r="AD38" s="105"/>
-      <c r="AE38" s="105"/>
+      <c r="AD38" s="103"/>
+      <c r="AE38" s="103"/>
       <c r="AF38" s="57"/>
       <c r="AG38" s="57"/>
       <c r="AH38" s="58"/>
       <c r="AI38" s="68"/>
       <c r="AJ38" s="69"/>
-      <c r="AK38" s="105"/>
-      <c r="AL38" s="105"/>
+      <c r="AK38" s="103"/>
+      <c r="AL38" s="103"/>
       <c r="AM38" s="57"/>
       <c r="AN38" s="57"/>
       <c r="AO38" s="58"/>
@@ -5149,15 +5146,15 @@
       <c r="AA40" s="58"/>
       <c r="AB40" s="98"/>
       <c r="AC40" s="99"/>
-      <c r="AD40" s="105"/>
-      <c r="AE40" s="105"/>
+      <c r="AD40" s="103"/>
+      <c r="AE40" s="103"/>
       <c r="AF40" s="57"/>
       <c r="AG40" s="57"/>
       <c r="AH40" s="58"/>
       <c r="AI40" s="53"/>
       <c r="AJ40" s="54"/>
-      <c r="AK40" s="105"/>
-      <c r="AL40" s="105"/>
+      <c r="AK40" s="103"/>
+      <c r="AL40" s="103"/>
       <c r="AM40" s="57"/>
       <c r="AN40" s="57"/>
       <c r="AO40" s="58"/>
@@ -5222,15 +5219,15 @@
       <c r="AA41" s="58"/>
       <c r="AB41" s="100"/>
       <c r="AC41" s="61"/>
-      <c r="AD41" s="105"/>
-      <c r="AE41" s="105"/>
+      <c r="AD41" s="103"/>
+      <c r="AE41" s="103"/>
       <c r="AF41" s="57"/>
       <c r="AG41" s="57"/>
       <c r="AH41" s="58"/>
       <c r="AI41" s="59"/>
       <c r="AJ41" s="60"/>
-      <c r="AK41" s="105"/>
-      <c r="AL41" s="105"/>
+      <c r="AK41" s="103"/>
+      <c r="AL41" s="103"/>
       <c r="AM41" s="57"/>
       <c r="AN41" s="57"/>
       <c r="AO41" s="58"/>
@@ -5291,15 +5288,15 @@
       <c r="AA42" s="58"/>
       <c r="AB42" s="101"/>
       <c r="AC42" s="102"/>
-      <c r="AD42" s="105"/>
-      <c r="AE42" s="105"/>
+      <c r="AD42" s="103"/>
+      <c r="AE42" s="103"/>
       <c r="AF42" s="57"/>
       <c r="AG42" s="57"/>
       <c r="AH42" s="58"/>
       <c r="AI42" s="68"/>
       <c r="AJ42" s="69"/>
-      <c r="AK42" s="105"/>
-      <c r="AL42" s="105"/>
+      <c r="AK42" s="103"/>
+      <c r="AL42" s="103"/>
       <c r="AM42" s="57"/>
       <c r="AN42" s="57"/>
       <c r="AO42" s="58"/>
@@ -5332,11 +5329,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>89</v>
+        <v>90.5</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5358,7 +5355,7 @@
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5611,10 +5608,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="116"/>
+      <c r="B2" s="114"/>
       <c r="C2" s="78" t="s">
         <v>14</v>
       </c>
@@ -5623,11 +5620,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="113" t="str">
+      <c r="A3" s="111" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="114"/>
+      <c r="B3" s="112"/>
       <c r="C3" s="79">
         <f>Zeitplanung!C9</f>
         <v>4</v>
@@ -5640,31 +5637,31 @@
       <c r="F3" s="80"/>
     </row>
     <row r="4" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="113" t="str">
+      <c r="A4" s="111" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="114"/>
+      <c r="B4" s="112"/>
       <c r="C4" s="79">
         <f>Zeitplanung!C14</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D4" s="79">
         <f>Zeitplanung!D14</f>
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="E4" s="81"/>
       <c r="F4" s="80"/>
     </row>
     <row r="5" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113" t="str">
+      <c r="A5" s="111" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="114"/>
+      <c r="B5" s="112"/>
       <c r="C5" s="79">
         <f>Zeitplanung!C18</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5" s="79">
         <f>Zeitplanung!D18</f>
@@ -5674,11 +5671,11 @@
       <c r="F5" s="80"/>
     </row>
     <row r="6" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="113" t="str">
+      <c r="A6" s="111" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="114"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="79">
         <f>Zeitplanung!C31</f>
         <v>6</v>
@@ -5690,11 +5687,11 @@
       <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="str">
+      <c r="A7" s="111" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="114"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="79">
         <f>Zeitplanung!C36</f>
         <v>0</v>
@@ -5706,11 +5703,11 @@
       <c r="F7" s="80"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="113" t="str">
+      <c r="A8" s="111" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="114"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="79">
         <f>Zeitplanung!C39</f>
         <v>8</v>

</xml_diff>

<commit_message>
set up flutter app
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidkapka/blj-notewriter/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D3B4E0-9EBC-0641-9557-43748A2B4821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AA2E7F-6A6C-C749-AD3C-514A5EEFBFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1505,6 +1505,21 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1535,21 +1550,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="48" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1657,7 +1657,7 @@
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
@@ -1725,13 +1725,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2238,8 +2238,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2558,88 +2558,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="106"/>
+      <c r="D7" s="110"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="107" t="s">
+      <c r="G7" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="107"/>
-      <c r="I7" s="107"/>
-      <c r="J7" s="107"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="107"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="107" t="s">
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="107"/>
-      <c r="P7" s="107"/>
-      <c r="Q7" s="107"/>
-      <c r="R7" s="107"/>
-      <c r="S7" s="107"/>
-      <c r="T7" s="108"/>
-      <c r="U7" s="107" t="s">
+      <c r="O7" s="111"/>
+      <c r="P7" s="111"/>
+      <c r="Q7" s="111"/>
+      <c r="R7" s="111"/>
+      <c r="S7" s="111"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="V7" s="107"/>
-      <c r="W7" s="107"/>
-      <c r="X7" s="107"/>
-      <c r="Y7" s="107"/>
-      <c r="Z7" s="107"/>
-      <c r="AA7" s="108"/>
-      <c r="AB7" s="109" t="s">
+      <c r="V7" s="111"/>
+      <c r="W7" s="111"/>
+      <c r="X7" s="111"/>
+      <c r="Y7" s="111"/>
+      <c r="Z7" s="111"/>
+      <c r="AA7" s="112"/>
+      <c r="AB7" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="AC7" s="107"/>
-      <c r="AD7" s="107"/>
-      <c r="AE7" s="107"/>
-      <c r="AF7" s="107"/>
-      <c r="AG7" s="107"/>
-      <c r="AH7" s="108"/>
-      <c r="AI7" s="107" t="s">
+      <c r="AC7" s="111"/>
+      <c r="AD7" s="111"/>
+      <c r="AE7" s="111"/>
+      <c r="AF7" s="111"/>
+      <c r="AG7" s="111"/>
+      <c r="AH7" s="112"/>
+      <c r="AI7" s="111" t="s">
         <v>49</v>
       </c>
-      <c r="AJ7" s="107"/>
-      <c r="AK7" s="107"/>
-      <c r="AL7" s="107"/>
-      <c r="AM7" s="107"/>
-      <c r="AN7" s="107"/>
-      <c r="AO7" s="108"/>
-      <c r="AP7" s="109" t="s">
+      <c r="AJ7" s="111"/>
+      <c r="AK7" s="111"/>
+      <c r="AL7" s="111"/>
+      <c r="AM7" s="111"/>
+      <c r="AN7" s="111"/>
+      <c r="AO7" s="112"/>
+      <c r="AP7" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="AQ7" s="107"/>
-      <c r="AR7" s="107"/>
-      <c r="AS7" s="107"/>
-      <c r="AT7" s="107"/>
-      <c r="AU7" s="107"/>
-      <c r="AV7" s="108"/>
-      <c r="AW7" s="107" t="s">
+      <c r="AQ7" s="111"/>
+      <c r="AR7" s="111"/>
+      <c r="AS7" s="111"/>
+      <c r="AT7" s="111"/>
+      <c r="AU7" s="111"/>
+      <c r="AV7" s="112"/>
+      <c r="AW7" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="AX7" s="107"/>
-      <c r="AY7" s="107"/>
-      <c r="AZ7" s="107"/>
-      <c r="BA7" s="107"/>
-      <c r="BB7" s="107"/>
-      <c r="BC7" s="108"/>
-      <c r="BD7" s="109" t="s">
+      <c r="AX7" s="111"/>
+      <c r="AY7" s="111"/>
+      <c r="AZ7" s="111"/>
+      <c r="BA7" s="111"/>
+      <c r="BB7" s="111"/>
+      <c r="BC7" s="112"/>
+      <c r="BD7" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="BE7" s="107"/>
-      <c r="BF7" s="107"/>
-      <c r="BG7" s="107"/>
-      <c r="BH7" s="107"/>
-      <c r="BI7" s="107"/>
-      <c r="BJ7" s="110"/>
+      <c r="BE7" s="111"/>
+      <c r="BF7" s="111"/>
+      <c r="BG7" s="111"/>
+      <c r="BH7" s="111"/>
+      <c r="BI7" s="111"/>
+      <c r="BJ7" s="114"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -3068,7 +3068,7 @@
       </c>
       <c r="D12" s="82">
         <f>SUM(G12:BJ12)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -3078,7 +3078,9 @@
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="63"/>
+      <c r="K12" s="63">
+        <v>0.25</v>
+      </c>
       <c r="L12" s="57"/>
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
@@ -3511,11 +3513,11 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3667,7 +3669,7 @@
       </c>
       <c r="D20" s="82">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3677,7 +3679,9 @@
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="94"/>
+      <c r="K20" s="94">
+        <v>2</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
@@ -3738,11 +3742,11 @@
         <v>57</v>
       </c>
       <c r="C21" s="49">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D21" s="82">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E21" s="50">
         <v>1</v>
@@ -3752,7 +3756,9 @@
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-      <c r="K21" s="94"/>
+      <c r="K21" s="94">
+        <v>5</v>
+      </c>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
@@ -4141,7 +4147,7 @@
       <c r="Y26" s="56"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
-      <c r="AB26" s="115"/>
+      <c r="AB26" s="106"/>
       <c r="AC26" s="84"/>
       <c r="AD26" s="103"/>
       <c r="AE26" s="103"/>
@@ -4214,8 +4220,8 @@
       <c r="Y27" s="56"/>
       <c r="Z27" s="57"/>
       <c r="AA27" s="58"/>
-      <c r="AB27" s="116"/>
-      <c r="AC27" s="115"/>
+      <c r="AB27" s="107"/>
+      <c r="AC27" s="106"/>
       <c r="AD27" s="103"/>
       <c r="AE27" s="103"/>
       <c r="AF27" s="57"/>
@@ -4283,7 +4289,7 @@
       <c r="Y28" s="56"/>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
-      <c r="AB28" s="115"/>
+      <c r="AB28" s="106"/>
       <c r="AC28" s="84"/>
       <c r="AD28" s="103"/>
       <c r="AE28" s="103"/>
@@ -4352,8 +4358,8 @@
       <c r="Y29" s="56"/>
       <c r="Z29" s="57"/>
       <c r="AA29" s="58"/>
-      <c r="AB29" s="117"/>
-      <c r="AC29" s="118"/>
+      <c r="AB29" s="108"/>
+      <c r="AC29" s="109"/>
       <c r="AD29" s="103"/>
       <c r="AE29" s="103"/>
       <c r="AF29" s="57"/>
@@ -5329,11 +5335,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>90.5</v>
+        <v>88.5</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>5</v>
+        <v>12.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5355,7 +5361,7 @@
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>8.25</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5608,10 +5614,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="114"/>
+      <c r="B2" s="118"/>
       <c r="C2" s="78" t="s">
         <v>14</v>
       </c>
@@ -5620,28 +5626,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="111" t="str">
+      <c r="A3" s="115" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="112"/>
+      <c r="B3" s="116"/>
       <c r="C3" s="79">
         <f>Zeitplanung!C9</f>
         <v>4</v>
       </c>
       <c r="D3" s="79">
         <f>Zeitplanung!D9</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="E3" s="81"/>
       <c r="F3" s="80"/>
     </row>
     <row r="4" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="111" t="str">
+      <c r="A4" s="115" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="112"/>
+      <c r="B4" s="116"/>
       <c r="C4" s="79">
         <f>Zeitplanung!C14</f>
         <v>2.5</v>
@@ -5654,28 +5660,28 @@
       <c r="F4" s="80"/>
     </row>
     <row r="5" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="111" t="str">
+      <c r="A5" s="115" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="112"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="79">
         <f>Zeitplanung!C18</f>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="79">
         <f>Zeitplanung!D18</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E5" s="81"/>
       <c r="F5" s="80"/>
     </row>
     <row r="6" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="str">
+      <c r="A6" s="115" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="112"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="79">
         <f>Zeitplanung!C31</f>
         <v>6</v>
@@ -5687,11 +5693,11 @@
       <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="111" t="str">
+      <c r="A7" s="115" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="112"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="79">
         <f>Zeitplanung!C36</f>
         <v>0</v>
@@ -5703,11 +5709,11 @@
       <c r="F7" s="80"/>
     </row>
     <row r="8" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="111" t="str">
+      <c r="A8" s="115" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="112"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="79">
         <f>Zeitplanung!C39</f>
         <v>8</v>

</xml_diff>

<commit_message>
Taking photos works now
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidkapka/blj-notewriter/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AA2E7F-6A6C-C749-AD3C-514A5EEFBFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DF0D8A-774D-6B42-954B-8307209231A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1140,7 +1140,7 @@
     </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1550,6 +1550,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2239,7 +2242,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3742,7 +3745,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="49">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D21" s="82">
         <f t="shared" si="0"/>
@@ -3764,7 +3767,7 @@
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
       <c r="P21" s="93"/>
-      <c r="Q21" s="93"/>
+      <c r="Q21" s="96"/>
       <c r="R21" s="56"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
@@ -3819,7 +3822,7 @@
         <v>50</v>
       </c>
       <c r="C22" s="49">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D22" s="82">
         <f t="shared" si="0"/>
@@ -3838,13 +3841,14 @@
       <c r="M22" s="58"/>
       <c r="N22" s="59"/>
       <c r="O22" s="60"/>
-      <c r="P22" s="96"/>
+      <c r="P22" s="93"/>
+      <c r="Q22" s="119"/>
       <c r="R22" s="93"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="93"/>
+      <c r="W22" s="96"/>
       <c r="X22" s="96"/>
       <c r="Y22" s="97"/>
       <c r="Z22" s="57"/>

</xml_diff>

<commit_message>
note editing in progress
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidkapka/blj-notewriter/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE34DAD-B894-DC41-883A-E25293A8ABBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C487CB-F01A-AB44-9651-2DCD0B653362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1734,7 +1734,7 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2241,8 +2241,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="D20" s="82">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3692,7 +3692,9 @@
       <c r="P20" s="93">
         <v>3</v>
       </c>
-      <c r="Q20" s="93"/>
+      <c r="Q20" s="93">
+        <v>3</v>
+      </c>
       <c r="R20" s="94"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
@@ -3830,7 +3832,7 @@
       </c>
       <c r="D22" s="82">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E22" s="50">
         <v>1</v>
@@ -3848,7 +3850,9 @@
       <c r="P22" s="93">
         <v>3</v>
       </c>
-      <c r="Q22" s="110"/>
+      <c r="Q22" s="110">
+        <v>5</v>
+      </c>
       <c r="R22" s="93"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
@@ -5349,7 +5353,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>20.25</v>
+        <v>28.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5395,7 +5399,7 @@
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
@@ -5681,7 +5685,7 @@
       </c>
       <c r="D5" s="79">
         <f>Zeitplanung!D18</f>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E5" s="81"/>
       <c r="F5" s="80"/>

</xml_diff>

<commit_message>
notes working, not saved yet
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidkapka/blj-notewriter/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C487CB-F01A-AB44-9651-2DCD0B653362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDD75CA-BA1F-DE46-94F0-696B7BD9D3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -2241,8 +2241,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
working on saving images to db
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidkapka/blj-notewriter/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8D9C03-B85F-B145-B105-1DAD13F00265}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435F8F80-2370-954F-94D5-776D44813F12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -389,7 +389,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +496,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="49">
     <border>
@@ -1140,7 +1146,7 @@
     </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1553,6 +1559,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1734,7 +1744,7 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.5</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2241,8 +2251,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3522,7 +3532,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>40.5</v>
+        <v>48.5</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3674,7 +3684,7 @@
       </c>
       <c r="D20" s="82">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3705,7 +3715,9 @@
       <c r="U20" s="59"/>
       <c r="V20" s="60"/>
       <c r="W20" s="96"/>
-      <c r="X20" s="93"/>
+      <c r="X20" s="93">
+        <v>2</v>
+      </c>
       <c r="Y20" s="94"/>
       <c r="Z20" s="57"/>
       <c r="AA20" s="58"/>
@@ -3913,11 +3925,11 @@
         <v>52</v>
       </c>
       <c r="C23" s="49">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D23" s="82">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>10</v>
       </c>
       <c r="E23" s="50">
         <v>1</v>
@@ -3944,12 +3956,14 @@
       <c r="W23" s="95">
         <v>4</v>
       </c>
-      <c r="X23" s="95"/>
-      <c r="Y23" s="97"/>
+      <c r="X23" s="95">
+        <v>3.5</v>
+      </c>
+      <c r="Y23" s="94"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
-      <c r="AB23" s="100"/>
-      <c r="AC23" s="61"/>
+      <c r="AB23" s="104"/>
+      <c r="AC23" s="95"/>
       <c r="AD23" s="64"/>
       <c r="AE23" s="64"/>
       <c r="AF23" s="57"/>
@@ -3964,7 +3978,7 @@
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
-      <c r="AR23" s="61"/>
+      <c r="AR23" s="95"/>
       <c r="AS23" s="61"/>
       <c r="AT23" s="56"/>
       <c r="AU23" s="57"/>
@@ -3992,7 +4006,7 @@
         <v>51</v>
       </c>
       <c r="C24" s="49">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D24" s="82">
         <f t="shared" si="0"/>
@@ -4019,7 +4033,7 @@
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
       <c r="W24" s="96"/>
-      <c r="X24" s="93"/>
+      <c r="X24" s="96"/>
       <c r="Y24" s="94"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
@@ -4039,7 +4053,7 @@
       <c r="AO24" s="58"/>
       <c r="AP24" s="59"/>
       <c r="AQ24" s="60"/>
-      <c r="AR24" s="55"/>
+      <c r="AR24" s="96"/>
       <c r="AS24" s="55"/>
       <c r="AT24" s="56"/>
       <c r="AU24" s="57"/>
@@ -4067,11 +4081,11 @@
         <v>56</v>
       </c>
       <c r="C25" s="49">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D25" s="82">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" s="50">
         <v>1</v>
@@ -4093,13 +4107,17 @@
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
       <c r="V25" s="60"/>
-      <c r="W25" s="96"/>
-      <c r="X25" s="96"/>
+      <c r="W25" s="93">
+        <v>1.5</v>
+      </c>
+      <c r="X25" s="93">
+        <v>1.5</v>
+      </c>
       <c r="Y25" s="97"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
-      <c r="AB25" s="104"/>
-      <c r="AC25" s="95"/>
+      <c r="AB25" s="106"/>
+      <c r="AC25" s="84"/>
       <c r="AD25" s="103"/>
       <c r="AE25" s="103"/>
       <c r="AF25" s="57"/>
@@ -4114,7 +4132,7 @@
       <c r="AO25" s="58"/>
       <c r="AP25" s="59"/>
       <c r="AQ25" s="60"/>
-      <c r="AR25" s="55"/>
+      <c r="AR25" s="120"/>
       <c r="AS25" s="55"/>
       <c r="AT25" s="56"/>
       <c r="AU25" s="57"/>
@@ -4146,7 +4164,7 @@
       </c>
       <c r="D26" s="82">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="E26" s="50"/>
       <c r="F26" s="51"/>
@@ -4166,10 +4184,12 @@
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
-      <c r="W26" s="55">
-        <v>4</v>
-      </c>
-      <c r="X26" s="55"/>
+      <c r="W26" s="93">
+        <v>2.5</v>
+      </c>
+      <c r="X26" s="93">
+        <v>1</v>
+      </c>
       <c r="Y26" s="56"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
@@ -4189,7 +4209,7 @@
       <c r="AO26" s="58"/>
       <c r="AP26" s="59"/>
       <c r="AQ26" s="60"/>
-      <c r="AR26" s="93"/>
+      <c r="AR26" s="96"/>
       <c r="AS26" s="55"/>
       <c r="AT26" s="56"/>
       <c r="AU26" s="57"/>
@@ -5365,7 +5385,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>44.25</v>
+        <v>52.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5439,7 +5459,7 @@
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
@@ -5697,7 +5717,7 @@
       </c>
       <c r="D5" s="79">
         <f>Zeitplanung!D18</f>
-        <v>40.5</v>
+        <v>48.5</v>
       </c>
       <c r="E5" s="81"/>
       <c r="F5" s="80"/>

</xml_diff>